<commit_message>
deleting to store again to remove lfs
</commit_message>
<xml_diff>
--- a/output/dbms comparision.xlsx
+++ b/output/dbms comparision.xlsx
@@ -1460,13 +1460,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A43" sqref="A43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="103.88671875" customWidth="1"/>
+    <col min="1" max="1" width="82.21875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">

</xml_diff>